<commit_message>
templates of protocols fix
</commit_message>
<xml_diff>
--- a/app/src/main/assets/protocol_referee.xlsx
+++ b/app/src/main/assets/protocol_referee.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexg\Desktop\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinov\AndroidStudioProjects\ATour\app\src\main\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>№</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>в сиреневую строчку вписывакм свои данные по образцу оранжевой строки</t>
-  </si>
-  <si>
-    <t>в протоколе группы местами не переставлять!!!</t>
   </si>
   <si>
     <t>Безроднов С.Б., МС, сс1к, Нижний Тагил</t>
@@ -81,7 +78,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -256,32 +253,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -601,8 +598,8 @@
   </sheetPr>
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:L8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,74 +611,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
+      <c r="A2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
       <c r="M2" s="6"/>
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
@@ -695,7 +692,7 @@
       <c r="C5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="15" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="12" t="s">
@@ -725,7 +722,7 @@
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
-      <c r="D6" s="18"/>
+      <c r="D6" s="16"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -1210,38 +1207,36 @@
       <c r="N32" s="1"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
     </row>
     <row r="34" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
     </row>
@@ -1279,6 +1274,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A33:L33"/>
+    <mergeCell ref="A34:L34"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A5:A6"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="H5:J5"/>
@@ -1290,11 +1290,6 @@
     <mergeCell ref="A4:L4"/>
     <mergeCell ref="A3:L3"/>
     <mergeCell ref="D5:D6"/>
-    <mergeCell ref="A33:L33"/>
-    <mergeCell ref="A34:L34"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>

</xml_diff>